<commit_message>
[Backend] Product > Beverage 로 연관된 테이블명 변경
</commit_message>
<xml_diff>
--- a/data/ProductData.xlsx
+++ b/data/ProductData.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hmnam/IdeaProjects/ToffeeStory/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFC56B6-8672-5C44-9AC1-814DC6B821D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B463E6B-4930-4A49-9FBD-BD1A59A049F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="5" r:id="rId1"/>
-    <sheet name="ProductTopping" sheetId="13" r:id="rId2"/>
+    <sheet name="BeverageTopping" sheetId="13" r:id="rId2"/>
     <sheet name="ToppingCategory" sheetId="8" r:id="rId3"/>
     <sheet name="Topping" sheetId="11" r:id="rId4"/>
     <sheet name="SubTopping" sheetId="12" r:id="rId5"/>
     <sheet name="QuantityType" sheetId="10" r:id="rId6"/>
     <sheet name="QuantityCode" sheetId="9" r:id="rId7"/>
-    <sheet name="ProductCategory" sheetId="6" r:id="rId8"/>
-    <sheet name="Product" sheetId="7" r:id="rId9"/>
+    <sheet name="BeverageCategory" sheetId="6" r:id="rId8"/>
+    <sheet name="Beverage" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -492,7 +492,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="264">
   <si>
     <t>Topping</t>
   </si>
@@ -788,9 +788,6 @@
     <t>애플 시나몬소스</t>
   </si>
   <si>
-    <t>productCategoryNo</t>
-  </si>
-  <si>
     <t>바닐라 플랫 화이트</t>
   </si>
   <si>
@@ -800,9 +797,6 @@
     <t>물</t>
   </si>
   <si>
-    <t>productCategoryName</t>
-  </si>
-  <si>
     <t>디카페인 스타벅스 돌체 라떼</t>
   </si>
   <si>
@@ -935,9 +929,6 @@
     <t>바닐라 크림 프라푸치노</t>
   </si>
   <si>
-    <t>productName</t>
-  </si>
-  <si>
     <t>망고 바나나 블렌디드</t>
   </si>
   <si>
@@ -1281,6 +1272,18 @@
   </si>
   <si>
     <t>subToppingNo(FK)</t>
+  </si>
+  <si>
+    <t>BeverageCategoryNo</t>
+  </si>
+  <si>
+    <t>BeverageCategoryName</t>
+  </si>
+  <si>
+    <t>BeverageNo</t>
+  </si>
+  <si>
+    <t>BeverageName</t>
   </si>
 </sst>
 </file>
@@ -1705,9 +1708,9 @@
   </sheetPr>
   <dimension ref="A1:AE1002"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScale="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V2" sqref="V2:AB68"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U58" sqref="U58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1942,10 +1945,10 @@
         <v>1</v>
       </c>
       <c r="AD3" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="AE3" s="14" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2034,7 +2037,7 @@
         <v>48</v>
       </c>
       <c r="AE4" s="14" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2120,7 +2123,7 @@
         <v>30</v>
       </c>
       <c r="AE5" s="14" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2207,7 +2210,7 @@
         <v>47</v>
       </c>
       <c r="AE6" s="16" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2267,7 +2270,7 @@
         <v>15</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="T7" s="1">
         <v>2</v>
@@ -2293,7 +2296,7 @@
         <v>5</v>
       </c>
       <c r="AD7" s="13" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AE7" s="14">
         <v>9</v>
@@ -2327,7 +2330,7 @@
         <v>6</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="4"/>
@@ -2382,7 +2385,7 @@
         <v>6</v>
       </c>
       <c r="AD8" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AE8" s="14">
         <v>10</v>
@@ -2483,7 +2486,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
@@ -2551,7 +2554,7 @@
         <v>9</v>
       </c>
       <c r="AD10" s="19" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2569,7 +2572,7 @@
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F11" s="1">
         <v>2</v>
@@ -2649,7 +2652,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F12" s="1">
         <v>2</v>
@@ -2717,7 +2720,7 @@
         <v>1</v>
       </c>
       <c r="AD12" s="13" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2791,7 +2794,7 @@
         <v>2</v>
       </c>
       <c r="AD13" s="20" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2833,7 +2836,7 @@
         <v>34</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="T14" s="1">
         <v>1</v>
@@ -2856,7 +2859,7 @@
         <v>3</v>
       </c>
       <c r="AD14" s="20" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2898,7 +2901,7 @@
         <v>34</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="T15" s="1">
         <v>2</v>
@@ -2924,7 +2927,7 @@
         <v>4</v>
       </c>
       <c r="AD15" s="20" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2966,7 +2969,7 @@
         <v>34</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="T16" s="1">
         <v>3</v>
@@ -3057,7 +3060,7 @@
         <v>6</v>
       </c>
       <c r="AD17" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="3:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3083,7 +3086,7 @@
         <v>2</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="N18" s="1">
         <v>5</v>
@@ -3125,7 +3128,7 @@
         <v>7</v>
       </c>
       <c r="AD18" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="3:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3202,7 +3205,7 @@
         <v>18</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F20" s="1">
         <v>2</v>
@@ -3261,7 +3264,7 @@
         <v>9</v>
       </c>
       <c r="AD20" s="20" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="3:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3329,7 +3332,7 @@
         <v>10</v>
       </c>
       <c r="AD21" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="3:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3417,7 +3420,7 @@
         <v>3</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N23" s="1">
         <v>3</v>
@@ -3479,7 +3482,7 @@
         <v>3</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P24" s="6" t="str">
         <f t="shared" si="2"/>
@@ -3524,7 +3527,7 @@
         <v>23</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F25" s="1">
         <v>3</v>
@@ -3541,7 +3544,7 @@
         <v>3</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="P25" s="6" t="str">
         <f t="shared" si="2"/>
@@ -3554,7 +3557,7 @@
         <v>30</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="T25" s="1">
         <v>5</v>
@@ -3583,7 +3586,7 @@
         <v>24</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F26" s="1">
         <v>3</v>
@@ -3600,7 +3603,7 @@
         <v>3</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="P26" s="6" t="str">
         <f t="shared" si="2"/>
@@ -3624,7 +3627,7 @@
         <v>25</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F27" s="1">
         <v>3</v>
@@ -3641,7 +3644,7 @@
         <v>3</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="N27" s="1">
         <v>4</v>
@@ -3668,7 +3671,7 @@
         <v>26</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F28" s="1">
         <v>3</v>
@@ -3685,7 +3688,7 @@
         <v>3</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="P28" s="6" t="str">
         <f t="shared" si="2"/>
@@ -3712,7 +3715,7 @@
         <v>27</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F29" s="1">
         <v>3</v>
@@ -3729,7 +3732,7 @@
         <v>3</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="N29" s="1">
         <v>3</v>
@@ -3759,7 +3762,7 @@
         <v>28</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F30" s="1">
         <v>3</v>
@@ -3776,7 +3779,7 @@
         <v>3</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="P30" s="6" t="str">
         <f t="shared" si="2"/>
@@ -3800,7 +3803,7 @@
         <v>29</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F31" s="1">
         <v>3</v>
@@ -3845,7 +3848,7 @@
         <v>30</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F32" s="1">
         <v>3</v>
@@ -3862,7 +3865,7 @@
         <v>4</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N32" s="1">
         <v>0</v>
@@ -3892,7 +3895,7 @@
         <v>31</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F33" s="1">
         <v>4</v>
@@ -3940,7 +3943,7 @@
         <v>32</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F34" s="1">
         <v>4</v>
@@ -3957,7 +3960,7 @@
         <v>4</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="N34" s="1">
         <v>4</v>
@@ -3988,7 +3991,7 @@
         <v>33</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F35" s="1">
         <v>4</v>
@@ -4005,7 +4008,7 @@
         <v>4</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P35" s="6" t="str">
         <f t="shared" ref="P35:P53" si="5">"{ categoryNo: " &amp; L35 &amp; ", no: " &amp; K35 &amp; ", name: " &amp; CHAR(39) &amp; M35 &amp; CHAR(39) &amp;", toppingPrice: 0, quantityType: 1 },"</f>
@@ -4033,7 +4036,7 @@
         <v>34</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F36" s="1">
         <v>4</v>
@@ -4050,7 +4053,7 @@
         <v>5</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P36" s="6" t="str">
         <f t="shared" si="5"/>
@@ -4081,7 +4084,7 @@
         <v>35</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F37" s="1">
         <v>4</v>
@@ -4098,7 +4101,7 @@
         <v>5</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="N37" s="1">
         <v>3</v>
@@ -4132,7 +4135,7 @@
         <v>36</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F38" s="1">
         <v>4</v>
@@ -4149,7 +4152,7 @@
         <v>5</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="N38" s="1">
         <v>2</v>
@@ -4177,7 +4180,7 @@
         <v>37</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F39" s="1">
         <v>4</v>
@@ -4194,7 +4197,7 @@
         <v>5</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="N39" s="1">
         <v>5</v>
@@ -4222,7 +4225,7 @@
         <v>38</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F40" s="1">
         <v>5</v>
@@ -4239,7 +4242,7 @@
         <v>5</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N40" s="1">
         <v>1</v>
@@ -4270,7 +4273,7 @@
         <v>39</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F41" s="1">
         <v>5</v>
@@ -4287,7 +4290,7 @@
         <v>5</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N41" s="1">
         <v>1</v>
@@ -4318,7 +4321,7 @@
         <v>40</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F42" s="1">
         <v>5</v>
@@ -4335,7 +4338,7 @@
         <v>6</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N42" s="1">
         <v>0</v>
@@ -4363,7 +4366,7 @@
         <v>41</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F43" s="1">
         <v>5</v>
@@ -4380,7 +4383,7 @@
         <v>6</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="N43" s="1">
         <v>6</v>
@@ -4411,7 +4414,7 @@
         <v>42</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F44" s="1">
         <v>5</v>
@@ -4459,7 +4462,7 @@
         <v>43</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F45" s="1">
         <v>5</v>
@@ -4507,7 +4510,7 @@
         <v>44</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F46" s="1">
         <v>5</v>
@@ -4524,7 +4527,7 @@
         <v>8</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="N46" s="1">
         <v>1</v>
@@ -4555,7 +4558,7 @@
         <v>45</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F47" s="1">
         <v>5</v>
@@ -4605,7 +4608,7 @@
         <v>46</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F48" s="1">
         <v>5</v>
@@ -4656,7 +4659,7 @@
         <v>47</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F49" s="1">
         <v>5</v>
@@ -4701,7 +4704,7 @@
         <v>48</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F50" s="1">
         <v>5</v>
@@ -4718,7 +4721,7 @@
         <v>10</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="N50" s="1">
         <v>5</v>
@@ -4746,7 +4749,7 @@
         <v>49</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F51" s="1">
         <v>6</v>
@@ -4763,7 +4766,7 @@
         <v>11</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N51" s="1">
         <v>4</v>
@@ -4793,7 +4796,7 @@
         <v>50</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F52" s="1">
         <v>6</v>
@@ -4810,7 +4813,7 @@
         <v>11</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="N52" s="1">
         <v>7</v>
@@ -4840,7 +4843,7 @@
         <v>51</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F53" s="1">
         <v>6</v>
@@ -4857,7 +4860,7 @@
         <v>11</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="N53" s="1">
         <v>7</v>
@@ -4887,7 +4890,7 @@
         <v>52</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F54" s="1">
         <v>6</v>
@@ -4904,7 +4907,7 @@
         <v>11</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="N54" s="1">
         <v>7</v>
@@ -4931,7 +4934,7 @@
         <v>53</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F55" s="1">
         <v>7</v>
@@ -4975,7 +4978,7 @@
         <v>54</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F56" s="1">
         <v>7</v>
@@ -5008,7 +5011,7 @@
         <v>55</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F57" s="1">
         <v>7</v>
@@ -5040,7 +5043,7 @@
         <v>56</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F58" s="1">
         <v>7</v>
@@ -5072,7 +5075,7 @@
         <v>57</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F59" s="1">
         <v>8</v>
@@ -5104,7 +5107,7 @@
         <v>58</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F60" s="1">
         <v>8</v>
@@ -5133,7 +5136,7 @@
         <v>59</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F61" s="1">
         <v>8</v>
@@ -5165,7 +5168,7 @@
         <v>60</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F62" s="1">
         <v>8</v>
@@ -5194,7 +5197,7 @@
         <v>61</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F63" s="1">
         <v>8</v>
@@ -5226,7 +5229,7 @@
         <v>62</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F64" s="1">
         <v>8</v>
@@ -5258,7 +5261,7 @@
         <v>63</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F65" s="1">
         <v>8</v>
@@ -5290,7 +5293,7 @@
         <v>64</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F66" s="1">
         <v>8</v>
@@ -5319,7 +5322,7 @@
         <v>65</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F67" s="1">
         <v>8</v>
@@ -5348,7 +5351,7 @@
         <v>66</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F68" s="1">
         <v>8</v>
@@ -5377,7 +5380,7 @@
         <v>67</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F69" s="1">
         <v>8</v>
@@ -5397,7 +5400,7 @@
         <v>68</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F70" s="1">
         <v>8</v>
@@ -5417,7 +5420,7 @@
         <v>69</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F71" s="1">
         <v>9</v>
@@ -5437,7 +5440,7 @@
         <v>70</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F72" s="1">
         <v>9</v>
@@ -5457,7 +5460,7 @@
         <v>71</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F73" s="1">
         <v>9</v>
@@ -12910,8 +12913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FBBF88E-2FBC-4041-9C90-8A7986A8A028}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12923,7 +12926,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="34" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B1" s="33" t="s">
         <v>6</v>
@@ -12932,10 +12935,10 @@
         <v>7</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F1" s="33" t="s">
         <v>46</v>
@@ -12962,7 +12965,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
@@ -14111,7 +14114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5CF5AC-37A2-824E-86DA-7674868D8B47}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="142" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -14127,10 +14130,10 @@
         <v>8</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -14198,7 +14201,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C7" s="6" t="str">
         <f t="shared" si="0"/>
@@ -14274,7 +14277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EEA344-AEB0-5C48-9E7C-A9EDEA7173C5}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="135" workbookViewId="0">
+    <sheetView topLeftCell="A39" zoomScale="135" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
@@ -14286,13 +14289,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D1" t="s">
         <v>56</v>
@@ -14316,7 +14319,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
@@ -14333,7 +14336,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
@@ -14350,7 +14353,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -14367,7 +14370,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -14384,7 +14387,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
@@ -14401,7 +14404,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
@@ -14418,7 +14421,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
@@ -14435,7 +14438,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
@@ -14452,7 +14455,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
@@ -14469,7 +14472,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
@@ -14486,7 +14489,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="32" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
@@ -14503,7 +14506,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="32" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
@@ -14520,7 +14523,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="32" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
@@ -14537,7 +14540,7 @@
         <v>5</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
@@ -14554,7 +14557,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="32" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
@@ -14565,13 +14568,13 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D17">
         <v>5</v>
       </c>
       <c r="F17" s="32" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
@@ -14588,7 +14591,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="32" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
@@ -14605,7 +14608,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="32" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
@@ -14622,7 +14625,7 @@
         <v>5</v>
       </c>
       <c r="F20" s="32" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
@@ -14639,7 +14642,7 @@
         <v>2</v>
       </c>
       <c r="F21" s="32" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
@@ -14650,13 +14653,13 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D22">
         <v>3</v>
       </c>
       <c r="F22" s="32" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
@@ -14667,13 +14670,13 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="F23" s="32" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
@@ -14684,13 +14687,13 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="F24" s="32" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
@@ -14701,13 +14704,13 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="F25" s="32" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
@@ -14718,13 +14721,13 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D26">
         <v>4</v>
       </c>
       <c r="F26" s="32" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
@@ -14735,13 +14738,13 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
@@ -14752,13 +14755,13 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D28">
         <v>3</v>
       </c>
       <c r="F28" s="32" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
@@ -14769,13 +14772,13 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
@@ -14792,7 +14795,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
@@ -14803,13 +14806,13 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="F31" s="32" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
@@ -14826,7 +14829,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
@@ -14837,13 +14840,13 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D33">
         <v>4</v>
       </c>
       <c r="F33" s="32" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
@@ -14854,13 +14857,13 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="F34" s="32" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
@@ -14871,13 +14874,13 @@
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="F35" s="32" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
@@ -14888,13 +14891,13 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D36">
         <v>3</v>
       </c>
       <c r="F36" s="32" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
@@ -14905,13 +14908,13 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D37">
         <v>2</v>
       </c>
       <c r="F37" s="32" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
@@ -14922,13 +14925,13 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D38">
         <v>5</v>
       </c>
       <c r="F38" s="32" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
@@ -14939,13 +14942,13 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="F39" s="32" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
@@ -14956,13 +14959,13 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="F40" s="32" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
@@ -14973,13 +14976,13 @@
         <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="F41" s="32" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
@@ -14990,13 +14993,13 @@
         <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D42">
         <v>6</v>
       </c>
       <c r="F42" s="32" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
@@ -15013,7 +15016,7 @@
         <v>4</v>
       </c>
       <c r="F43" s="32" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
@@ -15030,7 +15033,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="32" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
@@ -15041,13 +15044,13 @@
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D45">
         <v>1</v>
       </c>
       <c r="F45" s="32" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
@@ -15064,7 +15067,7 @@
         <v>4</v>
       </c>
       <c r="F46" s="32" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
@@ -15081,7 +15084,7 @@
         <v>3</v>
       </c>
       <c r="F47" s="32" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
@@ -15098,7 +15101,7 @@
         <v>3</v>
       </c>
       <c r="F48" s="32" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
@@ -15109,13 +15112,13 @@
         <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D49">
         <v>5</v>
       </c>
       <c r="F49" s="32" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
@@ -15126,13 +15129,13 @@
         <v>11</v>
       </c>
       <c r="C50" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D50">
         <v>4</v>
       </c>
       <c r="F50" s="32" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
@@ -15143,13 +15146,13 @@
         <v>11</v>
       </c>
       <c r="C51" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D51">
         <v>7</v>
       </c>
       <c r="F51" s="32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
@@ -15160,13 +15163,13 @@
         <v>11</v>
       </c>
       <c r="C52" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D52">
         <v>7</v>
       </c>
       <c r="F52" s="32" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
@@ -15177,7 +15180,7 @@
         <v>11</v>
       </c>
       <c r="C53" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D53">
         <v>7</v>
@@ -15209,7 +15212,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScale="163" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15313,7 +15316,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D6" s="7">
         <v>2</v>
@@ -15439,7 +15442,7 @@
         <v>34</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D13" s="7">
         <v>1</v>
@@ -15457,7 +15460,7 @@
         <v>34</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D14" s="7">
         <v>2</v>
@@ -15476,7 +15479,7 @@
         <v>34</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D15" s="7">
         <v>3</v>
@@ -15638,7 +15641,7 @@
         <v>30</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D24" s="7">
         <v>5</v>
@@ -15666,10 +15669,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="23" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -15685,7 +15688,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
@@ -15693,7 +15696,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
@@ -15701,7 +15704,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
@@ -15709,7 +15712,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
@@ -15725,7 +15728,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
@@ -15733,7 +15736,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
@@ -15749,7 +15752,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
@@ -15757,7 +15760,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -15782,7 +15785,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>59</v>
@@ -15796,10 +15799,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
@@ -15810,7 +15813,7 @@
         <v>48</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
@@ -15821,7 +15824,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
@@ -15832,7 +15835,7 @@
         <v>47</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
@@ -15840,10 +15843,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
@@ -15851,10 +15854,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -15867,7 +15870,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="192" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15879,13 +15882,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>260</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>261</v>
       </c>
       <c r="C1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -16005,8 +16008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B66780-C3AA-D543-B091-4AF43DC4518F}">
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView zoomScale="141" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -16018,16 +16021,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>6</v>
+        <v>262</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>147</v>
+        <v>263</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>98</v>
+        <v>260</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -16140,7 +16143,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" s="7">
         <v>2</v>
@@ -16155,7 +16158,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C10" s="7">
         <v>2</v>
@@ -16170,7 +16173,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C11" s="7">
         <v>2</v>
@@ -16290,7 +16293,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C19" s="7">
         <v>2</v>
@@ -16365,7 +16368,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C24" s="7">
         <v>3</v>
@@ -16380,7 +16383,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C25" s="7">
         <v>3</v>
@@ -16395,7 +16398,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C26" s="7">
         <v>3</v>
@@ -16410,7 +16413,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C27" s="7">
         <v>3</v>
@@ -16425,7 +16428,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C28" s="7">
         <v>3</v>
@@ -16440,7 +16443,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C29" s="7">
         <v>3</v>
@@ -16455,7 +16458,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C30" s="7">
         <v>3</v>
@@ -16470,7 +16473,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C31" s="7">
         <v>3</v>
@@ -16485,7 +16488,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C32" s="7">
         <v>4</v>
@@ -16500,7 +16503,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C33" s="7">
         <v>4</v>
@@ -16515,7 +16518,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C34" s="7">
         <v>4</v>
@@ -16530,7 +16533,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C35" s="7">
         <v>4</v>
@@ -16545,7 +16548,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C36" s="7">
         <v>4</v>
@@ -16560,7 +16563,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C37" s="7">
         <v>4</v>
@@ -16575,7 +16578,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C38" s="7">
         <v>4</v>
@@ -16590,7 +16593,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C39" s="7">
         <v>5</v>
@@ -16605,7 +16608,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C40" s="7">
         <v>5</v>
@@ -16620,7 +16623,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C41" s="7">
         <v>5</v>
@@ -16635,7 +16638,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C42" s="7">
         <v>5</v>
@@ -16650,7 +16653,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C43" s="7">
         <v>5</v>
@@ -16665,7 +16668,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C44" s="7">
         <v>5</v>
@@ -16680,7 +16683,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C45" s="7">
         <v>5</v>
@@ -16695,7 +16698,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C46" s="7">
         <v>5</v>
@@ -16710,7 +16713,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C47" s="7">
         <v>5</v>
@@ -16725,7 +16728,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C48" s="7">
         <v>5</v>
@@ -16740,7 +16743,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C49" s="7">
         <v>5</v>
@@ -16755,7 +16758,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C50" s="7">
         <v>6</v>
@@ -16770,7 +16773,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C51" s="7">
         <v>6</v>
@@ -16785,7 +16788,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C52" s="7">
         <v>6</v>
@@ -16800,7 +16803,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C53" s="7">
         <v>6</v>
@@ -16815,7 +16818,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C54" s="7">
         <v>7</v>
@@ -16830,7 +16833,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C55" s="7">
         <v>7</v>
@@ -16845,7 +16848,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C56" s="7">
         <v>7</v>
@@ -16860,7 +16863,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C57" s="7">
         <v>7</v>
@@ -16875,7 +16878,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C58" s="7">
         <v>8</v>
@@ -16890,7 +16893,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C59" s="7">
         <v>8</v>
@@ -16905,7 +16908,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C60" s="7">
         <v>8</v>
@@ -16920,7 +16923,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C61" s="7">
         <v>8</v>
@@ -16935,7 +16938,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C62" s="7">
         <v>8</v>
@@ -16950,7 +16953,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C63" s="7">
         <v>8</v>
@@ -16965,7 +16968,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C64" s="7">
         <v>8</v>
@@ -16980,7 +16983,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C65" s="7">
         <v>8</v>
@@ -16995,7 +16998,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C66" s="7">
         <v>8</v>
@@ -17010,7 +17013,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C67" s="7">
         <v>8</v>
@@ -17025,7 +17028,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C68" s="7">
         <v>8</v>
@@ -17040,7 +17043,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C69" s="7">
         <v>8</v>
@@ -17055,7 +17058,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C70" s="7">
         <v>9</v>
@@ -17070,7 +17073,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C71" s="7">
         <v>9</v>
@@ -17085,7 +17088,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C72" s="7">
         <v>9</v>

</xml_diff>

<commit_message>
[Backend] Products 엔티티 JsonReference 추가
</commit_message>
<xml_diff>
--- a/data/ProductData.xlsx
+++ b/data/ProductData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hmnam/IdeaProjects/ToffeeStory/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B463E6B-4930-4A49-9FBD-BD1A59A049F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E65063C-F86A-BD4D-B40B-D982EB37B7E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16009,7 +16009,7 @@
   <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>